<commit_message>
Renamed Shiksha module to Pariksha
</commit_message>
<xml_diff>
--- a/open-commons-ofds/Ofds_Features_Links.xlsx
+++ b/open-commons-ofds/Ofds_Features_Links.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RESTServices" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
   <si>
     <t xml:space="preserve">Module Name</t>
   </si>
@@ -962,7 +962,7 @@
   </sheetPr>
   <dimension ref="A1:AA243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -970,7 +970,7 @@
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.24"/>
@@ -3022,13 +3022,13 @@
   </sheetPr>
   <dimension ref="A1:AA241"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.26"/>
@@ -3371,7 +3371,9 @@
       <c r="C10" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
gconfig app migrated to thymeleaf
</commit_message>
<xml_diff>
--- a/open-commons-ofds/Ofds_Features_Links.xlsx
+++ b/open-commons-ofds/Ofds_Features_Links.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RESTServices" sheetId="1" state="visible" r:id="rId2"/>
@@ -81,8 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">API(service/junit)
+Audit Log (History)
 errorMsgLang=Hi,Bn
-Create Master Data - NA
+Create Master Data (FlyWay) - NA
 Postman Request
 UI Integrated
 JMX for PT - NA
@@ -962,15 +963,15 @@
   </sheetPr>
   <dimension ref="A1:AA243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.24"/>
@@ -1016,7 +1017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3022,13 +3023,13 @@
   </sheetPr>
   <dimension ref="A1:AA241"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.26"/>

</xml_diff>